<commit_message>
16/08/2023 Major stuff completed in the JulyMonthData project got a way to handle Sub Cats
</commit_message>
<xml_diff>
--- a/Data-Science/Projects/Live-Project/TheOneMonth/July2023ExpenseReport.xlsx
+++ b/Data-Science/Projects/Live-Project/TheOneMonth/July2023ExpenseReport.xlsx
@@ -339,6 +339,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -346,6 +347,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -437,10 +439,10 @@
       <sheetName val="Details"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
@@ -710,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F112"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="F116" sqref="F116"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2706,13 +2708,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D112">
-        <f>SUM(D2:D111)</f>
-        <v>340034</v>
-      </c>
-    </row>
   </sheetData>
+  <conditionalFormatting sqref="C31">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>